<commit_message>
added spar test cases
</commit_message>
<xml_diff>
--- a/testconfig/testdata/testdata.xlsx
+++ b/testconfig/testdata/testdata.xlsx
@@ -1,36 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4FC262-1242-46A5-AF7D-35DA224BD9FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583E6868-CF68-44CD-94A1-3EBBD127C723}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6345" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6345" firstSheet="20" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resetPassword" sheetId="1" r:id="rId1"/>
     <sheet name="loginTest" sheetId="2" r:id="rId2"/>
     <sheet name="groupProgramCreation" sheetId="5" r:id="rId3"/>
     <sheet name="eligibilityManagerCreation" sheetId="18" r:id="rId4"/>
-    <sheet name="deduplicationManagerCreation" sheetId="19" r:id="rId5"/>
-    <sheet name="cashPaymentManagerCreation" sheetId="21" r:id="rId6"/>
-    <sheet name="dbtPaymentManagerCreation" sheetId="22" r:id="rId7"/>
-    <sheet name="gsmaMoneyPaymentManagerCreation" sheetId="23" r:id="rId8"/>
-    <sheet name="voucherConfigFileCreation" sheetId="24" r:id="rId9"/>
-    <sheet name="deduplicationManagerMapping" sheetId="20" r:id="rId10"/>
-    <sheet name="registryIDTypeCreation" sheetId="6" r:id="rId11"/>
-    <sheet name="groupCreation" sheetId="3" r:id="rId12"/>
-    <sheet name="registrantTagCreation" sheetId="7" r:id="rId13"/>
-    <sheet name="genderTypeCreation" sheetId="8" r:id="rId14"/>
-    <sheet name="groupTypeCreation" sheetId="9" r:id="rId15"/>
-    <sheet name="groupMembershipKindCreation" sheetId="10" r:id="rId16"/>
-    <sheet name="individualProgramCreation" sheetId="14" r:id="rId17"/>
-    <sheet name="groupProgramFundCreation" sheetId="15" r:id="rId18"/>
-    <sheet name="individualProgramFundCreation" sheetId="16" r:id="rId19"/>
-    <sheet name="relationshipsCreation" sheetId="11" r:id="rId20"/>
-    <sheet name="idTypeCreation" sheetId="12" r:id="rId21"/>
-    <sheet name="individualCreation" sheetId="4" r:id="rId22"/>
-    <sheet name="unarchiveGroup" sheetId="13" r:id="rId23"/>
+    <sheet name="eligibilityManagerMapping" sheetId="25" r:id="rId5"/>
+    <sheet name="deduplicationManagerCreation" sheetId="19" r:id="rId6"/>
+    <sheet name="cashPaymentManagerCreation" sheetId="21" r:id="rId7"/>
+    <sheet name="dbtPaymentManagerCreation" sheetId="22" r:id="rId8"/>
+    <sheet name="gsmaMoneyPaymentManagerCreation" sheetId="23" r:id="rId9"/>
+    <sheet name="voucherConfigFileCreation" sheetId="24" r:id="rId10"/>
+    <sheet name="deduplicationManagerMapping" sheetId="20" r:id="rId11"/>
+    <sheet name="registryIDTypeCreation" sheetId="6" r:id="rId12"/>
+    <sheet name="groupCreation" sheetId="3" r:id="rId13"/>
+    <sheet name="registrantTagCreation" sheetId="7" r:id="rId14"/>
+    <sheet name="genderTypeCreation" sheetId="8" r:id="rId15"/>
+    <sheet name="groupTypeCreation" sheetId="9" r:id="rId16"/>
+    <sheet name="groupMembershipKindCreation" sheetId="10" r:id="rId17"/>
+    <sheet name="individualProgramCreation" sheetId="14" r:id="rId18"/>
+    <sheet name="groupProgramFundCreation" sheetId="15" r:id="rId19"/>
+    <sheet name="individualProgramFundCreation" sheetId="16" r:id="rId20"/>
+    <sheet name="relationshipsCreation" sheetId="11" r:id="rId21"/>
+    <sheet name="idTypeCreation" sheetId="12" r:id="rId22"/>
+    <sheet name="individualCreation" sheetId="4" r:id="rId23"/>
+    <sheet name="unarchiveGroup" sheetId="13" r:id="rId24"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
   <si>
     <t>username</t>
   </si>
@@ -152,21 +153,12 @@
     <t>Auto2</t>
   </si>
   <si>
-    <t>amountPerCycle</t>
-  </si>
-  <si>
     <t>autouser@gmail.com</t>
   </si>
   <si>
     <t>openg2p@123</t>
   </si>
   <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>Group Voucher Program</t>
-  </si>
-  <si>
     <t>Group Cash Program</t>
   </si>
   <si>
@@ -182,12 +174,6 @@
     <t>Individual Cash Program</t>
   </si>
   <si>
-    <t xml:space="preserve">Individual DBT Program </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual GSMA Money Program </t>
-  </si>
-  <si>
     <t>Individual DBT Program</t>
   </si>
   <si>
@@ -197,18 +183,9 @@
     <t>eligibilityManagerName</t>
   </si>
   <si>
-    <t>Voucher Eligibility Manager (Group)</t>
-  </si>
-  <si>
     <t>Cash Eligiblity Manager (Group)</t>
   </si>
   <si>
-    <t>DBT Eligibility Manager (Group)</t>
-  </si>
-  <si>
-    <t>GSMA Money Eligibility Manager (Group)</t>
-  </si>
-  <si>
     <t>deduplicationManagerName</t>
   </si>
   <si>
@@ -275,23 +252,41 @@
     <t>GL_Qrcode</t>
   </si>
   <si>
+    <t>Individual G2P Connect Program</t>
+  </si>
+  <si>
+    <t>Voucher Eligibility Manager(Individual)</t>
+  </si>
+  <si>
+    <t>Cash Eligiblity Manager (Individual)</t>
+  </si>
+  <si>
+    <t>G2P Connect Eligibility Manager(Individual)</t>
+  </si>
+  <si>
+    <t>Voucher Deduplication Manager(Individual)</t>
+  </si>
+  <si>
+    <t>Cash Deduplication Manager (Group)</t>
+  </si>
+  <si>
+    <t>Cash Deduplication Manager (Individual)</t>
+  </si>
+  <si>
+    <t>G2P Connect Deduplication Manager(Individual)</t>
+  </si>
+  <si>
     <t>{
-                "iss": "{{ user.env['ir.config_parameter'].sudo().get_param('web.base.url') }}/api/v1/payments",
-                "sub": "{{ object.id }}",
-                "aud": "{{ object.service_provider_id.id }}",
-                "exp": {{ object.valid_until.strftime("%s") if object.valid_until else "null" }},
-                "iat": {{ object.valid_from.strftime("%s") if object.valid_from else datetime.datetime.utcnow().strftime("%s") }},
                 "amount": "{{ object.initial_amount }}",
                 "type": "voucher",
                 "code": "{{ object.code }}",
                 "bName": "{{ object.partner_id.name }}",
                 "bAddress": "{{ object.partner_id.address }}",
-                "spName": "{{ object.service_provider_id.name }}",
-                "docs": {{ "[" + ",".join([ '"' + docs.slug + '"' for docs in object.supporting_document_ids.filter_for_tags_any(['Medical Prescription', 'Medical Diagnosis']) ]) + "]" }}
+                "spName": "{{ object.service_provider_id.name }}",              
             }</t>
   </si>
   <si>
-    <t>&lt;html&gt;
+    <t xml:space="preserve">&lt;html&gt;
                 &lt;body&gt;
                     &lt;meta name="pdfkit-title" content="Guarantee Letter"/&gt;
                     &lt;meta name="pdfkit-page-size" content="A4"/&gt;
@@ -305,10 +300,6 @@
                     &lt;/style&gt;
                     &lt;header&gt;
                         &lt;div style="position:absolute;top:1in;left:1in;"&gt;
-                            &lt;a href="http://www.dswd.gov.ph"&gt;
-                                &lt;img name="dswdlogo" src="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMUAAABMCAYAAADdh3PgAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAAAJcEhZcwAADsMAAA7DAcdvqGQAAB+RSURBVHhe7V0HmFxV2R41ydbZ2ZnZ2Wm3zGzvZWan3ZkkGEJIIcmmQUilpCe7qaTtJpvN1imrsQCKICJ2UWyoKKCCotgRxZ8iIopINsaQX+ng/333njNzZ+be2QTRJ+t/3+f5nnPn3O8932nfKbeNToMGDRo0aNCgQYMGDRo0aNCgQYMGDRo0aNCgQYMGDRo0aNCgQYMGDRo0aNCgQYMGDRo0aNCgQYMGDRo0aNDw78aaNUWXvDBe/czZUzX/lKSWhErynzkH+fnmnq35LMliEuaaK+s4YfRhV3jsn1Tc4TiEKKm45G8h8bwrHLuTExIf5cOxj/Ch+NWWxh2tOn5mPknyPMDnmxq31jO+Y12cEPsoLyS+AnJKbg/S/6UrHL0V7TG+vhmWxq5KnW5uHkkgDSa+s54LjPwKeW5MI0LyDCEfjH2cqKWjuMrCBob+RO1l8SBPxVVXW4h2GqxNW59V5EH9OJv3M3qHz8z4+4+6IgmIo+eoZPOgPt/khdgjWBeu0NitfCS+zdqyM2CsWGEgJicvJKeo+cPZ8ZrHz4xXfx3Cu1DosVqcUryajlocPaa/IR/fAvkzyN3d3UaOZDEJW3P3d6RGwYaTJOUUqTj6243HVJ+EvBB/hgvFhhwdx2tJshOivHpVBRcYfo9LiP/WJcTePBd70Gle44T4z8HWPkPrzlKSVBLWpm33q+UT8niPsWFTVvmLbTOWgv2/qfMSP3W07Gkn6mlweg4Rp8jK56tcaHSo1H35QrA7nnIKDKko20vTQR7kDfLwead/6N1g8h2S5UkI4hTPvHCqehS9PFNm63SGUaPxbZcVkG6mrQJTMwN5+SI6hdJMYW3e+RupMVKjWIXYYOlx9HcFHlN9GQ8a7lW3EHueCY40k6RVYeBWGUH/eyCvS2mepz0h8RLINyCptE5SVndtTI0Htn5pbtrUQVSTMNWsvgk67hs5eK84PD3riXoS00qbFsC5M0o8cIozbHB0s55dsEhyCjh3PuWjIuOBrdPOcHweMT/5sG514RxYrvwB5BhUyoep5+OoACPddf0lxktPcfX/PMU3gECIx0mBOHI8ztX95RRT95Nxtu7lNB0V3ud0une5QvFb5fZ05kV6yMdnQRRnCmtz96PSSJYScfRSEWlkI78VeHw4/qzD1x8iyWfD2lLEBodgSZTOk/+WSy57LiE6otP1vZOkrCvl5m2n5zJ50Kl+Y2nbIxBViqn2tr13JNNT4GHI+Ad3gG7SDqLA1LACynpWiQfxf+YDw/OnFbsWp2YKZclZPgUeG45frqtSXj5e0CBO8YzkFIkPUc/HCkCnGCgxzhU7Ne3caaIUlynKPHQKXHvL7cmdQmmmsLdQpyCjE+FJjZCKo7+lNTA5p8CDTvA6rIs/a669xkFMpKG8edvut9MeF0okO3qBTejgg4OKPGiHvzu9h9cRVYLieoj/kZSeuj2sUwM/M225Vuru3AHcF5V44BSPWRq2VU3Tu2QzBUkzKdm8ZEhFgYfp8aFEJ8nG5EG6U8hnijhUcGz/uc4U2eeIqPCyZ4q43Clgo21UWD6hU+AULXEoT5q2U3H0t9iBqb4aT4i/xPr7MjqgBGfH0cdy2WMDx+91dvR+wOnt/SDTceQ2PjT6TC57fCh6N0laBOM9RM7J9Eno8BzaTtREFLMLpkN7/FZKT9JR4kEbPmyt3ewiNBHmqlWfgvjkXkjOg+XTz1An5RSp9FOSzUuGVBR4MODAZjzxebt3T5mYkcmC5J4iY6bAtfP5LJ/emlOMgVOk7KWcQm1PsYs4RWo0kq/xueDISUf7vsdtLV0g3U+4hcRz0OiviLq5eOHEfabq5U5iRkSBxbsc6uOMEg8a+3UmODhGVJMwMAuWgL0/i7rKvKft3r4IUdc52/adls7J9EkIZblOp1vxLqKqM1Wt3EXTovlWW+OXN+9O2yuVN2z8ghqPC8fuQ530mSKVFuXx4cRZxnuY1G3X41xw6FmsHxBxr6XKExInOf8gbCEn0cYbneKM4kwh31NgxyYiOoKCqJ1T4UnLpxgsn1L20mcKNadIjUSUR4+dbQe7iSoib6qhoc3kXrab8fXDBl2dh8L4+uYSngjJKeLgFOl6Ik+IP+f0HFlAVOUohQ6Do/LrSjzcw8jtwPJsNJkm1SchONDXCtjZdFmnZ/3H30fToqLEQ+H8w2sJD1DgZAOD36XnUOQ8aIONqJU+U2QL5P0TYnIE04r5+mmG2mUOz8HbcbZV44kixG/BCxaEeuGD3qeQnCJ7T5GaKRpBMkd8iKPHqjOFMi9zpkB7EzrFBHsKe/u+LqKaBn3ZjGo2OPi0Gg+FF8biRF1EscW/Qpopsu2hs7CBoa1ENQ2Flo6rgfd3cSQWUuIWYrB8Gj3L+fqTjmup37hVShPSpnZICPn5aiF3qZ2oMngFi+aB5lttjc8FE9cTnk43RS/APuNRNR4XiW5CtYn2FJlOkUKJqbxuw11UL5MnhkLitK2tq4EQLnykO0UcnAILkoApVnKKf+dGW76nQHsTbbSlS7KSvpxHjxkVp0DYmnYcUeOJEor/gqiKkJwie6agPD4Uv5vx9DbrTHNLdLqWIkKDzlVXU1a3XuxoE8HARYyucExKk9ohIdj+nblpRx3qFVlDTTBzPEXzQEWJhwLcF0UDgCnF7unglGQvIomcR9SoU5yUpyMXdafAgcDfygYGXlXioaA9u+ewh6hf+Mg9UyRSG20XdG4XhGkjPi6FyHHWOSIqvLc0U+DyaTpWNB2JJJ5U+TBTtO2VL5/SYDBE8H7DX5V4VIiqiHyLN8yHEqdy2YP0XuXC8fug093p8PVtsTd3LTbXru3Q6WZOIcnkhtFrgM33KXHkpnZk9sqat3pRrazumgU0ThJJR42HYmnYZ0OugbtsA+Tzf6X4dB7sE55FHURyppie0ktJbqdAlDdsIpeL03kYoj1+enwLUb3wkb7Rxj2FVCC8WvKf3GijPeIUn1HbaNuTV59SFZ+6GqS+fCIo4sNjX1biUSF6FNPsLbv/mMteSshvWCbw4eiTfDB2DycM9zk6erLKkIECLjh8p9hJqR2ZPbvnoOgUzo7DCRonSdLen2Fjf1Y8zsgntKXYCUvYhQdS8ZIOtQez3ftRBzHxRju3U5TVroX9UTYPQ7THhaM3ENULH9mXZKUC0Zmir8QyN1fnTh6/BafIcZ9CZaYAp8gYEdNmitxOUYANq8SjIr/agzBXrtwOnfwNuY4STz4iykduGKGf58KJI7CeVnweCZDPhYZvy+TRdLE9UInxH0sOHpJIOuDkh/hI7F4xLqNe2FCiH2csNjh2PBUv6VB7mDcxF4B/daYwVly+MtspZPYiiRuJ6oWPDKfI2FMk9g9YKoVxpvaZca7+9bdj+XSSrfvHSabut33QYDBSfUluD9fnkA+YKdT2FN059xQTOkUofrsSjwosha4lukk4vb3JK2QoSjwq4jmFNT4sr37PevsvIUnK8c7yuqs3qfGwPfAuOCfe5EvFk3Mvu4IjXYy/T3r0I6Ne3LCvKHWt4nHvI49HofasrfsbST5kM0W6LhWsO6KqjGJvGR8aVuSSOpvEToGVAuIG4SOJn3YEjizb2rJp4QMV4Z2nbdynJEdQEJwR1OJBxtn6M89x9R/6etXFqze2bd7nCQ7ACBb/m9xe+kZb7eadpC/n0eNzmikUeFTAKXqJbhL5pfU8bIY/TXWUeFRynYOynuRCQxeTZJPQ22bNU+NBfr/N+o43iiNw1rnYU/bWfXP0zhnroN1eyTwPnJfZ4PB6Dp0i4xy1J9/7iI95hIlTKMhEM4WuuKZMdF4FrmhvEjtF2h1tbAwchWCUeBJGu/cuZ3YXJGouK3vY7b/xaa75TycnuCQ7Dk7xe771l7+q7Bj4YMOK4tbg8cuhMR/CNKU1sGSL2jun5ZMCT+w0cHxuy6dsHhVeiPUQ3XQU28ucHT2DXCj6NyUe/S0urWj+FPLJCbFHWU9PJUlVRLHN3wB2f6zGcwmxPiV7UIcPGBu3Qh3x+WxgRLoELNcRYq9ywdgtXCj2mpyHIeaTC8d+Ll8upj/7pGDvXJwiNJDFw1BacsYmj1NkX5KV1oPyO74pETffn6wPDm/Z3LZ58Y31nZd/v0L4yjhb97txvu7voiOwdadBfgPxN19ft2TdxvbtixpCQ7fxwthjuZ6yRHvpM4XK1ScFHs3nxMunBCyfsnlUYFSV3fTKhoGbN8vasOmLXGjkIRgoyLsUKFI6E5UPOv9pxj+QuUSrdAsJ8kh8Ns8txH6l1A5Qli8Rvs7WvPMPCrw3wN7v5HHyfMK5m4GavMuccoqUnpyHdUdUFVHgnMnwwkgWD0OxXiarU0Cn6KZenmtEhFnjTRjxn6kVRj493X9k3+Xtu5fdXDVn2YeY9qtPVM27bLWn+8h0X2+0KhS7H0aYs5SXaySFke2J1NUntZmCPjqe4qXNFDkuyQLS9hRK5dMxywuIbm7kO1hjxRXzLA1bDkKanzmX8lF7fCh6uxnKSVJC6B1t18GyNTdPHgd19RLU6yHC15mr15w4Jx75Lc4UoWjaUpE4BblPkc2baE9RVr1mU057k+nqE3EK8dFx+Dm1vKlrNYwiz09UqbQRwDleg8o8DQ41yITiTdBg+CLOSxD3ei6evBHZUPSOsrpdePeWOoXKo+N0pqDppjd+7pmCmXD5RBTPB/iIdr5e7zMzgcFtrtDo75XKh5K0J8R/aKxcl9zgIoz84mMT8mRx0D7/6xISVxC6zsAvvsgViaXpTNR+tqbdMwldRPpGO5s30fIpdUk2nYfhZHUKcaYgUbBMWOh2dhz9BlT+GaXpULqkJx3TkAslHuSFxCOpxsjN4yMxmG3iP3G0H7gGb2IR0zlnCvE+BbVLRG4vl1MU22eWqfGoEFUCe2G+sYHLM7S68kvbeQO/qN1cufoiUWpXKj5qXlTUUm737LsF6uE1tXzCuYdKa69Ke2Cv1HnpTqiPF0XdHOWjAu0ybm09kPYkLBvoS9PJ1Q7gUGdsjd0+QhWRXD6Jl2SzeRM5hbWl61Nq9rDd2WDf5UT1wofoFCfTnUJEkdta3rzjSuy49CoCFaWrJVw4/iDMGo/kugJDz0Ga47hxL7bNrifWKCSnOJnjjrYsPXmaKLmWT7bmHSvUeCiQp+8TVYDRYGu77ijG4ciOAsfPUh7MiNuIYjZKGkwOz6EfydOmPAyhjn5UXrOuhWiLmFLsmgHpP5HJQcnMJwrWNaEm4fQcekCuo8RLSjh+j7FibdpMLM4Uua8+qS6f8o1eTu3KEwrmxdKws42oX/hQdQqCPENzBRceG4NpkFw+Bc/HzRjeLJKFfHjsB3wYZopkZcC5pKR4fCT+pNOzP6jTVSm9kSVttE/muE9B7RKR28vlFGxw8AU1niiyS4ZTplj9MHI/IsYr2IMRVeZA2TBVLj+klk+oo6yZQjfV2ggd/Reibo7yUYEOmtxPUNhbd10v11Hi0d/A/6axcnFa/SadAmcKBR7kW9Up7G37b1TjiWE48W21F7kuSEjLJ+kxDxKlCEvN+rmwbn6STodigWVhavmEv8m5pMBvIfES23HsfcU1V+Z64YQsn2qUZ4oJn5I9IF8+TdUV1tmL+c56xtd/Vy4e5Pvl8qZ9qdF7ankLGxr6mairwAP9pznPcfERDCXYWvZI9wYyeGgPHOoBU/XazBlSZ23dJT0FmyOfVJyBoTWEloS59tqL5DpKPPqbDQzsIbQkUnuKlJ6cl3X1qZC35VlmVkGdX4/1p8YTQ9ik6x2dZsK88CG/T0GiVGFt3nYdFlSscBzRZCFstMEpYPkkVkS2QIX/miSTC9JMkevmHbVLRG6PCw5/0962Z8DatH3A4T18wo0fHIjEnhfP5+BB3n5grLgsbTlhbdoGjR2HvUE2D+Jf4UOxj5XVraaPdidhci+dzQaGXlCzxwVHb9XZvYVEPYmyuqtuhXTfyJVPKoSShmllvhrgj1MdJR4VxndsL6ElkXSKDPtUsG2dnoNi3drb9g1w4dH7QP+JpI4qL37K2XF8KTEzOYAzBX3JiESpwtq4BZwCRyHwfjqikZAXYPmUY6aAc+fqFDke86AvGaXSVrMnnYPjjHxSkfMY/7HrIPm0J1v1tsgayDMsuZR5cO5FPhT9ltPbu9vh2b/V0X5wC9tx9CO8MHoSzr2pxIOO9bzT349voWWh2B6+FmfTCcsXSqQ94i6DlRMSX1fliSLm+wlH+6GsO+sTzRQY5qpP1RlGGLvH1r6XJ2YmB5SuPqkhzSnoVRISTnT1Cc6d50yh4hTncHVGftUjM59UkAed9E3YRN9Z5L7WSkykweE5+PDbaY8TYj+3N3RnXWpGFFgCy6CO/jGRPZiRhwglE8WMf/iEGk8SsR0esbbsDRBOEqmZQtLL5GGYq3xKPKjfM1xgSHyzb1Jh3eqSc18+NW7ejyOCuNHG6+mykAuDU4gbbfxNz1E5L6dQnynEPUV62mr2pHOpY0VeOPqctXXvRST5LBjZzggXGnkji5eR1rnac3b0qi8jChtsjO+o9E54Bk8eZ/f2JN/xzoSpauU1ajxJ8NJq4l6lTW9yo030MnkY5iqfUhw4WdrbjJMG57rRRpTXb+pkYWSVJCZJePROJhS/mwvH70Sn4ELRu1lhVNLBT1YSYWXP7ucAmSmUN9r2FnLzTlbxb7WTwij2OOR7JUlaFU7v4QNy3lu1B3WQ9nUOJdhbdp7O5GXaK62/RnUpkm9siMBo/VslniTgFJGxzxH1NLzdTgEOsVtnvST5RuKkAt1TnDlVFR86VGTNJSdOzLKe+MjCtyxDQ02K6VL58uetjWdOVj2qNlPYmrsfnHDNLYr0O3MNDLPV69BYf2UDIx/QNayYRpKdCFO5wOAm2D88hfzztPcaPkzJ+EZWkbRyoryxezhX+SC9z5qq8PVXVTRzQvyhTF5ShPhLkMZhopuGaXp+Ppw7KXbqTB75nVk+uQ4MiHgz9iyk8VNYxl0JSaZ9kG1SYd2VJf6z49VffeFU9Y9BfvLCqVoMyXFaCFIjj5PFq/LIsSKPHGfzxv9YNbh1lSHr6w/59tkcExjADxv/mAqMjD8RjzGUH9Nz5Bg20zfam3ces1SuqSLJnRf0jktrrS27BvnACD7l+2upo6SL2BFFZ4g9Ana/D8uhI4aaNW6SxIQodS1dmywDKQdsvpPlgT3JsNKVKxmKHO0HhjN5NC2Yze+DPcksopuBcitwb4LOncWjx2lpyuLZwNAtjvZ9J8rqNs40cAsmz1c71MAwuoL58/P5zrl5lReKzJypy/ogcRIljCmvpLHyfIWw/2XkGaorim2RBmPllZemy9pLLeTYVH1FPT4aQijnAUOpUt6p6Iqa8IJA7u8nFdssSlxRDDXgoKmPLGTDVKLIm0CAeG7vpGvQoEGDBg0aNGj4r0SeocXt9BzpZnw9vXZvT9aL+28F0gN/bx3Wmg1uncmvepUFN6/Ott51JcxykxhhXqS3e3p3Mr7eI+ba7RM+eIYfF2M7erMeqiurWjvT6e1Nfmy5rPZq8QFDvUOoZTy9q0ymuSXGmlVhe8aHvfBxcqi/1cbKq1jW17PV6elR2cz+6yhhZvmdnsPJ+jVXrVjDeI/0gt09zrbrqkn0OaPQ0mCztR9M+2To240SZk6V1bpm8lyeLSr3XsIL8dsc7XtX4lUENjD4CfyGaYFtZoeR75ynM9fq8bkaA7+s3cgvnZ9nCOBz/NPwfKl78UJdSdCkM3BGk3vJJZa6dXM4f/9fuFD0hiL3Qqu5YvHFRn7JXDO/tA65Jey7YVNmLYJK8pe6lyzAjp9naa8ycEs8aCvP4qm0t+zq4oT4z/XuK2qkHOrelVfCVppcnXOKrDOb4HcefoOWD8WP0e+TMh2HR7AMzlB0kAHBONzoYv70jnfjPxa9Ezep+LvUOafVXLv6Il6I3oaXZQtsHT6Mz7eHOXv7vn5I937kI2zNOx/mw7ElkPZxXog9xQrRDj4UwxeqFuC71QZ+6bsLLT6bvaV7kBcS3+OE6FFXOPoLPjwWtNRcGcE8F5ZNt+cbG1koXwjsTEd9WVmSmFbcWF/q7rwM6xl+lkj13TkPefB7CraBkVsatrXuGuZD0eSzS5b69feywYH1ds/Bbsj7Hbb2/eImX8/OXWhklzXmWYJVeudsdJZ36K0XBUpdS/nCsoAXwhk6fZ25sCzUzgVHr8f/4igwt0ObL51fbGuz5JeGeGNFZySVJ7M+mSdusYD8EnZRh07XMG2qoaUd9fSuRVDXenNJxSLsG9MN/OK2/DLfDJcQf5z19i+WcjwJUGjxz3EJiT48Nles7IDGfQhk1AUdmw1Gd0Mn6Gf8x/rYUPx2bAwulLiL9RyZzofjh1xC7NN8JB4vr9sUgjS+w4fGjkHcGeDe6ujoXQTpfE384BnqhRIHudDIGNPRdw1+6xQ6Wwwqa8TpPXqAExIJtxAbgI73Tfw7LOD9mj5Jio+ug96nuEgsAWncj2/3caGxG5jA8ZXYIKjj9PVsBM63WSH2NcifeJMM0vo8lgPsfAK/lseFxEu5H4ByRFnIC+TpZYdv2AwdaS+k/14Mxc4PNpCPgJlimI9gvhIfw2eO8ONwwHuF88fdoHcTG4pGIb/b8e/CkAd1MAxOgU+7tgLvBPx+L3S4E/gAHvDuxVdAIY2jbDAx4PQN3yL9Jx5Cb3b6jm2EetgAvAeKmIuboX4/Qez9ydFxaCU44hgbjG8RL/cKseRTrpa69ffq7JsKwYUtYA/qWSzPncDbCMe3Q957XOHEjYbmg0bG1/9LGFDWuELxj/CR6AehHsfKWrraIe0boB12oy4XSSRwUGMDsR6Ix0d3tkK9PIz/lwFteQPU5y7I27NcBAYALF9oZAXrP/ZFyBPoxW52ens2Q13cAdzl8PtnUn4Sv2cDA8k3BS944EyBDYXHBvscL1QAXof/GVQsvlJ6Bh8yw/MQfgwrHypsHBsVKuvHcP4HUPkvQUcUHN7e9+InUxjPwaexIkrdSxc62g/32Fp2rQXdAWPlskZI5xZsIDFtfHcbX9gPxQ/YWnYvkz7cNfgHaLRlwL8b70lgngodM9vAzod13k1T7W37HoW0DnPh2BFbU1fydUo20L+HC4x4He378ePGT3PBof3QID/CNMubNn+ai7ynAuyN63SbpvJ8X76zo2ct5OFlR0eChfAbKGAzCnbAKVIzBc5+mFco3xesrfsXwPnHobG/xQSjG+D4FbDxdwhfhLghCO8BG4egjJ8E/Yvh+G7Iy09p/WHauvxKFjhfwbJzwSjypc6db+RcERxU4u+Hc4+JTgEzobn2OgfU5xvgyDdhvvA7TbamnVE4Ts0U1CmKbRbIx5fA1hchz8+BnAa9J1n/8BxH24EvsNAGkJc+pz++HM69DHb+AXl6DTqw6BSQ149Zfb2NesdaM6wWnoC4T6JdO6QNbTuEdY7lMLXudkI7vInflBLjQCCdk65w/G9w/lGxrPghNpiFnZ7eJ/E33i+ytO1uJVm+8JFv8UawQrgIZB48nw3FDjLBgdUwcn+ODcfWQadfDA0IBUv8Av+uCcJvMMGRLi6cuB4rmQtHn4TzHkf7IfFFeEfrnrsg/gvYMRxte7dBp1wCaXfjFA6NFGWDI+u48NggVNR6aJilbDC22dK4/VLkwmjyIBccmY3PUZXXbhRfxMmzTne7gvE7uXC8F5Yl9zhCx9sh/a7yui3JdTWMsh+AMnwWv8+Eb7ZhHJQF8hnfATa+6vSPMi4h+kMmnIBGhFkH8g3x/wMzSyXwbuYjiR4ID2MnzXwMgg0efwpnOFzigcN+B3XK6q+q5sOJj0O51kLnmSXObjCy4z+Egv33QT2tB72bcVQGvZu4yFg35KcLZwQ2NNrPCWPLQOfDrG9UfFd7SoHVD/zPQDorII372UAigmW0Vmwph2Xt76A+tsOsfRzrEZ0Hzm0QMwcAp/gkL4wdh3KNQV4gjRHIz+h3mFCiE/Kw1eLrs5kqr4B6GHuMDxyvL7HPAkeHER5mIZh1Z1jrtzVC2Qeg3fsh/BqmDXm5nQ2MHIM0H4SZYxOGsLRGXld5U7cVlpVPFfLzbZhHaNOr2eDoXZCWD3VZYWQxxuMA5PAc/C5wd4DO3djeJMuTAaYSQ9WydpNrWQBDo3G2+L50qevy1vLmrsX4ckh5w9ajULgvQWeYjnsFfN/Z0rjhUvyYsMnd6ddZVhQb6cgOlWVt2rEA72zi3gR1TQz+IQpTAHEVOkNrqaFqZXt50/YlxfbLynDNjR8/Ri6+Bw2jez4ux5CHcYCpuL8oq984j9yNfoeYXtpGvCoPP0Jc3rxtsaFmuXgH2cAtdxc0bwnqK67E9fS7Sl3zecwXLsuQb3Yv8eFfB5trrpplbdgwC9a/LlPVEsZUtTztk/El7LwOuqEv5mfXow4cTsG6sjbsmGWsvII1OZcwuG8ys4scJVWduCR6J6yvAwZ+RRuu4dGeVAc4M8+yYl2j4G8Cvblm9cVYbkPlCm9K3zsV91/FVcsthZaZsBdZhn/JyxXyK8SPJyOKbYF6mh6WGeOKyoPNlsZNS03V15KXmRhTScUy+seSBabq5X5Lw7aI9Ec13kIsO7ZBWeUqL9Yhtrm5et1mcNw7wAFmlLqWwCjPFNA86Z0XQd4bpom/meUFBsclbfhcXFndhhpsF1LWd+D+DfNqrFweKqvbTveI/x0wVV0xBzaZuCbU7lz+P4HeMV+AmWc5OgGJ0qBBgwYNGjRo0KBBgwYNGjRo0KBBgwYNGjRo0KBBgwYNGjRo0KBBgwYNGjRo0KBBgwYNGjRo0KBBg4YLDTrd/wFt6pLp3NlN7AAAAABJRU5ErkJggg=="/&gt;
-                                &lt;img name="aicslogo" style="width: 69px; height: 79px" src="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAANoAAADwCAMAAABR9Iq5AAAC/VBMVEVHcEySJCPxpwCTHRyQfjQiPYwoRo0hPYyTHRzyqABJjCLWaAAndXsiPYzypwBJiiONGhfspgDyqADypwDxpwAiPYwiPYwhPYzypwBJjCMhPYySIR6PYCPupgAjQYryqAAiPIzxpgAiPYzooADvpgDwpwDxpwAiPYoiPYwjQ4M9aFzvpQDwpgDxpwD6qQAiPYxKiyIhQInyqADwpgDypwAiPYwiPYzypwAjP4rxpgDxpwBJjCPxpgDxpwAjPovzpwDmpgAjPosjPYslP4khPIxKhinypwDxpgDwowDypwDxpwDypwDxpwDwpgAjPoohPYxJiyMiPYyTHx3ypwDypwDyqADxpgDxpwDvpgCTHRwiPokkQYgiPYwiPovypwBLiiXxpwAiPopJiyMiPoolPYrypwAiPYxGiiVKMmRKiyMiQIqTHRzxpwAiPYwnQIQiP4oiPI1JiyNKiyNJiyNJjCNKiiXxpwCUHhvwpwDxqABKiyMhPYwiPYsiPYyTHRxKiSRKiyMiPYxKiiUlQIciPYxKiiQiPYtMiCiVIB1JiyPxpgDyqADwpwAiPYzypwAjP4rypwAiPYsiPYxKiyQiPYxJiyPxpwDyqABJiyMiPYztpgDupQCUIByVIhxKiyNShiZKiiSTHh1KiyNJiiWbKBrypwCTHRwiPIuTIxsiPIuTHxyUHxyTHRxKiyNJiyNJiiZJiiQiPYwiPYtJiiRKiiVLiiTxpwDxpwCUIRwiPYuTHRySHRxJiyNKiyNJiiTypwCUHxySHx2THRyTHRxWLVjwqABmKUmlOBavRhPxpwCUIh+2UBEiPYzDoAk3Z1NKiiOTHRxJiyNKiSVyJTyTHh2fLhjkkwPonAI9c0IxXGKUHhxJiyPCYg7Ocwq+XA9FhCwlRIMuV2qTHhzReAmUHxwpTHjcpARBezfWfwjKoQfJbAyGICndiQXTewl4JDfYgwffpAS+nwkoSH06alAqTXVKiyTyHSMiPY3yqACTHR1KjCPWowV/Ii/hpQPMoQcbN8qvAAAA9nRSTlMADvyuAfoG/v7+/gIC/PI7Cg3U/fbZ5M7hgN9iBx0Q7tWlfAosUuVVxwkEEDDdA479GLci6oZrxCxKgflNqFsTCDBgIcAKfcAG0HD4nTwo7u+jm4/YlDdBKPskHJg2yBDLgPRGUJnpGvrRQ8CLqQ08rZmzwKsURbJnrqOSTPP1GLuyOBTRcrUpE+hZc3nyvEBidJ5h98yisty8Fxk9J9Yuam/ief2E4Hcdi5JqzseTIVhlb4UzPmteMXjXc0ONU4dJVqRb/on+/f1pYvz0/vxI7E0v/nz8/f38/VFQ/fz8/f35gv15/Pn9/Pj9/vz8/fzUvedz7U8FYxENAAAXlUlEQVR42u1deVgUZ5r/gg1NQTcKcghRQNQGjHLJKYpcithyRaIBQeRQlyiggEaBhEMFUTzwxMQQIzHeB16JxiuZMZqJm2tzTjLJJjPZmZ2dvXcfmp7dfbaquqq6jq+qq7uqm24ffn8oVFcV9av3/d7re7+vARjFKEYxilGMYhSjGIVDI3XGtA97Zi9YtDNn3pNEK2LZg5VaHQlk5uGdzzwZxGbd0+jY8J677AkgdlirgwFJ2OTYxKac9NbxATkyy4GZLS3UCcHjhsJRmS3S6kxgi6dj2sXFiM4ksic5oiM7ohODCc87nszEMdPpNA5nTBbrxKLQwcKTRYhoaro9EY7ELEerMwMnHYiZ50xzmOmcchyH2hKzmOmQwlRHYTbVSWcmehyFWoy5zHQerziIDUHMpqZ74BjUjpjPTBfkEMnpJCcLqOkWOQK12ZYw02U7ADPFTIuoIVMdwPIjFlHTLbB/aj2WMdOteBKdmgFau0+43WMtpKaz+/LdLEuZ2b/5T7KY2ip7p3bDYmp77J3aSYupedk7tVUWU4u1d2qHLaYW5G7n1OZaTM1joZ1Tm/zkSm3xkzvWHlhMrdDeqe2ymFqWvVObZjG1w3afrllMze4LdqnellKbY9/EXukpRCylFpNkx9MaSydrdVIwc5edluw2ZSE6qQi6Z4dl5E0J0onhzTJL7Izc0iydbPCYbUdVkkmTx+vkhGafnfSTLNzloZMZyIoZdqGLXhyNkoGc07opI+6h17EmL8Zn7ZySbT6TpHvsIl/hCM8Cz2CJzGMVVrpPMttYotWshW+vZF7mdG8Ec1PFImZUFXSSMNzmzrDF4tcp2J5x5Yh1y3huYUrsJBVLTAoyj9rb5IXLmE4kaNrIMHueoYzaVXRX+7ZZKrmFduUcxl3H3xuJqkISQzJ7plpeR5jJiBwjbjBufMT2/vtDeiSs2cn2sakJ4uNG9qThK4eREWwrVNyj/XXkMKSBbJ6X2KARMkOTRJ9ZnWDT+dIIur5p4Dnkq4XimEGv9qS3icYutWFoRa+jxvBF6q+sFKONfLNqO2kjzsNmU28LaUZf28NvwqbMNWknC/mVbRbtzXjYqHE+giazWOH3+aFwoQQ5LJRVp9KU0tsmclPQxlm2qXDh+T1CbcemHDKt49zDFuNtnfFdxojwOdP4LGXQAtNXJxmTiFjrt18bO2+RxaIqUBHT9nATVURkhWeGcTnOzFetXRw25jAPRKfCs3oStIzOziU5YuOn540ebqV1M7gZlIYgs826cErO5geHj8TEzH1uV5JZr3+S0T3OtWZZYR71DhGb9R3RXL8V/6a7sZNnNrAZJlHv08l67m0Bxew5W4Z1syhbEmutUDmHMiFzbZpFKWZQQVeWdaYFnqEUI8vWRYtNTtadqaLaJmbavnR9g/SmWmsUKOeQd/fgu3t4bmVK/JX49Ja0QDPvveOd+0+fe+Pcr+6/9hTPGVSnTbb8GuM5gbz5TtjHgaElfgeHSKgD1vemifRCr7075q2iYRJFt94/9xos21hhPZVcItAA5xLabqRFQunbXGqa18+3XIfZcL31xWmumSRNifcsuY0UOZCzUzkCC1k9BIfSL2W60F2PvVg0DEfRmHc4IR45IGJkpkZWcbzZuWP4zbwhAfiE8t7znbWuw/xwHcPWSzKZQuSd9N5JvrJdrA8qfYaEoTxaDL3jU88WDQvj5S8mMkc76XwK5bQkC8m7rmC6zPAS9ZBJPB6E6eJbw6Zxnim4TeOt0Mq7CO5VioOHxEBZEM7W7y+KhsXg5fegnjVWvrLrFDKIW8c4vDdvSCTCtjIunPi+67A4FP2BUSOLld0BkH1XGsbbqjo4JBrBy2kXjls7LBquZ+nu8UO5xZZKCA3Zx2DmPGQGfKItYobiLL0Y4cVjzSzFPtKl0eP9vQeHzIJfLfl4Y8xiNuz6Bb0ORFhqjTxG0p14VUgS7WBi3pCZaFcZrjwLff7zZ984d+7dZyGxybAr3ZZksWfkpGUUxN0SaFpfC3NnzmElIVd642oC4NzK8Svfgzx80VnKyr8DcXcv03xADlkDkoUaWQanC62Aa+HD0ql4PzEOFnqp96Ifnf6Uy+yWIag6fZrP450fxxEbIkfJ9VUtd1lgqJJjAisZF9WWQ4ZiQCBQQEzIWkMic6yIkM6O81wzSdMhRL7G0B5uLhPoyxZZJNspg0SIOy8BT0NktsNwwbvDw78y/MSVbJExWFYQnRse0u2/wotrk86wBxkslKrN5KpkFVcdXY8Z6BxDzcvPxww6+VvOeFyr4NjrfZKpLUU4NcAMlrIp0+FJN5fb33CFNobQRobF4Krtb41eNlau1UXriOiRVvItYT1wJM+lWwNEULtvsJtMGb7HtSQK9hM5Sa3QuBMx/xHjoWiW0La5kJ/EqXHUURmP2iS1lw2Ji/sbZ1FJrT17jsh4OB7A9T7198l1tpulFvkJzaZNhYWw1HEv9Umk4cgL1IEak9TWUucazQiKW5wTXzQ+wEp5sm2iYBxkNCIqlpplAn5qiUpT1N6HU+MOtqLT7BTLW6KNTOB4kTrW44YKUAOZFlJ7kTso3zVOAjjJ0T3/DPcukawcOlyIWrwpas9Sp56jm0EItfOc9y1t4mEOV/as6PEoEKKWK57ajjHvTxSg5uq6gx1FeMlh+mkjdrkaZvnP+GAgsgFf/Bc88pq+WzQ1BiBSG36PbducJE0Br+BkfqEsoxePH13PjapSIDLmpfbeGwTu81OjBZIajtk2P7829H0gtGpPHJQBL7UwUdReoyKroh281Ix+gly1KWVrmaWE6aeV6DpZDNLloBbx87ME3lXwUvvUmORvlr7ibTPXObJz0F5ZFHLcDgIT+RWSZkeIlWRBEubtn+NMXLuw87BmQWouj8VQU+ygMoJPx/FSGzZmNguJRggJ879ZHK+2lVNixA/vd8ZAGE/8Z2fclZeKM/47br1M4PxEfmr3OZ4tyfJcTcN5ObmcggheNlBMx9BsOFSJ/4KffooZbv5aIBoxafxpwQqpTpZXyD3HcxZMl3IUb1DIZfsxz4VQmwgFlNo5Tq3V8nhkKrd6VMctMCr4qbHjzV9Dggw4TFBbJjX4J8KsuUBIarT4mE1Nwc6zWdRc6T+6sn8VojYJkRhqEbb/Hu1QGrRQxUMtXSlIreidcQK4LzTWFhrKbEEWUyM2+7pBO5QBKTDWKJjlIDI3LeZUmJnU3hLO7wXqIwAYmgacPCW6NXqoVquEcIsjP1yOg5i/3sqtMH8gidoxbnBrsWMjQjX6aisVrNavPKPiXpwBKUQyqX36NIbfMP6h/cahRm9LIBYkWdwgQzTSMWbm/aDznu3R7GtbYLXxD4YloGgcd4J0mcRghCH1GvhcRV68C/2s3BqY4jKpnR9jAqwC+S3IWLE4HCFKR4xlJTf5Jpl848j+ntqq9TzTih/Q+15Mxrbun0KKsQQeSMzYsiFm6AWB6fi8zILmkvXbCF5+akGprTX995lzNn+AGO+dllIzlPudGO3MgRyB5IUFQLUvfZBz+O8kUHM9Bikivi0nNVZyOaTudQGKvejUjZIbpXQKUTv/lEm8Bakzy0QNppCgnPm0IYb4K7OuNm09k10aqrxhR5U81FzFgC60tUBOhYSZEVDKeNiDxOw7ZhMUDOuZ54Imop2qcjWP1MzFG0BOM5IFdfn0wrgyk/5JGp11DXogGK1S9tIO/osEr3YayGn8YS4bgKvffPv3JLObjDAkkC6hFsy/d2IZuPHY/1jI681Hv2OVeCZzAyWpgRaKrii92x8//gUTRjsrKy+OpEQUgEWSvgXYFKKPJGquD3/4VyfOJGiMxEDrOfi0QYMew4+o8LjToc0ki1N4pRmvd1VaTu3Lj373NXTqOltieDwbPkd3WU/A7QDnklxCbGqsKeuUMo3pL8yh5orS+grhWzMRKzGp2Qz/JoHpJ0hujZxLoglqeajJrPXdZjiYQlL7J5Gs3nz0/Z++ZuyHwFq95ukkMRWdw9OisZ2kFnWX/RE566RGU4FmJVFbqH0smprrl4++/+evEaH19rSqjeUFBOIGCezj87spbhs+ufY6hWtjB376RW2Q2xlQpcwkI+CjhEF1FZLUw4++//1fnKArZ8fPgL90y8s+RLEuVsErNr3+Qr1ef6ixETMtUdvdsAH44x+/+fjjb3/6z//6D6oJsvyXn779+ONvfvz6qz/9+YePHj18+OWbBjx8+OjRRz/8+fd/+cpJ7CYJ9Bk2y4t1RIkV4bQxzKdGm357vz7qEnpkzUV99YCejvxrHMMDeX4x+0BoOetEJ0tuQs7iy2UPuBmetaHaTd9Yjx35PP+iW1R3o5FZxXXj6R381MSAK5xCqYVx0rFxe0bdDxme9bMT+qiO/EMbQeuJelRmV43Ukr+je3ni4P9atifmPL4pdgnTGYT1n8z9ZGyUgYC+PjlZXw3mN7QlR3UfSnYzKir97EvC1LwWzFmi4afG7X3ZJH0Sipg6nAn5aAM5oFCOV90bN1zV64/XGxy5G8fjvS5ATbMON38RmxbzbC2zIoIvlpDSpkVM+I6HCL6MsCSYH+i4qs9PRn/EZdZ9Gf2keyPj5Nt81IIWLzM++JRpWyAbC2in8toASd8lsoI/47trVL56t4YoyhmsAeg4PM6yOsSH/8Dcj2PLtFTWTedtzmKvT4csuJ2ilT5NTzZXLIZ91mS0hhe7DhDcqssAaNN3zydPMkjvIvEa/koLnbL2wdfTT9qVzdgkBtIbniRHbx3h9TWwZa9llHO7eDf56nGcW0UXzvkiZfXzcXNyqPECgxqycpdQz8fUk9SyVO+p/IZbWksMYWURaF50HU3csAfu317dfegObkPuYMf99Z9RzNAQBRVd/prbbkZqM2eb3KrBPee5WM5UCvXhBFlWUCcIrWO/Pn8NHWXJWFwCwHf66w0NDf6oh6jAwq8BcBn9+QIx1savWirOZEckxSC6I7BzycZaievYFgh+i8xxfb2/v//Vi+g//v36ruRqg6ZWlN2+fftzcD1fj4nVbaBpPmFJ/gr1kbxxXvYE6BfqLZGnaZBoh0LgKtTaiIrpmn9TI/rsd/u6kjcYDt8BTdXVn1xHZdZ3rZ9Q07JkA7WV4h9olgbazB+hkafVk/xCHb4vtus4AOpbOy4PzPff6N+VPEBEzwAl1IAxWwNaq9GY5RNg0EhsrAWtErUjRyrq5OAtuJt08jTokgW/CTwr9A80gL6u49UXL3VfQ6lR7qwfN4j9azDzj7q5ig7UARgt5IQHJso1EctWBekQni/TIKJ+reSF7+SY5QuyFWBgu77iGlC0NnUlU4FjNe7jWg2uDeWWPxbP8Si/hmT38Ie2M9bhJjAhFfrpPG/ZvmrDi9Myzsrd1hy4c7u1tbUeNSNXyYOYy6smg60yTG53DxiN/0wE3yMT6rMn9XghgtsR7JJvLRSR0DrxrfQu8yfRmtxGSz3RTAes6drYhdYjy9BxFtVPUZvsnqOBR1ponOXEt5MdxX2JVqaFJ9RyoSV8J6gGLt/ZgCOqwhBgfYZakAtlWHqQf1yPaWVZAz3QmoyrgsabiI/daYYDT8+wDEArsGvKrMPjeWI/c0Es8vLg20JJUTZARcp4YfK7ZIIZ+GT759txtvMbONSWeO7bg701ZMIDVEDumOHA/srcOQsT2Gs3uZHYXK0s+2otM7mzzn8nk9T60Emwu+hvDQbxkVJDubVhH/8fnRqmEYvw/VeR7Mm44dDuedvTEAGZ3F9Hnp2nyGVVAl9HeJwSmz8uszYi8v9soMOf/BFGDcXzZCiMrFz0KhncrbLVls77TG9V5E9yS/anMWOcwUMNfXU5qzTawpPGeCdhi812v0+dYPrLPy/SqnQYs4kHmurvkNU6xfWLjXgG9I8wariPZpQHUoHNQCxiCRKojbmjiWlUXx+WtOVvBO53+9xO9FdENeGZwLU2t4q+fIza39KoifviLpfc0rTirdbTT3zNeWyPoCeZ3uiPOrKNV1G739/YHdX4Omo6DpyIutDU1B916LPpQHW9wY1BLVZMoHRqN1ZmVx4MrrlZ52IVbjd0ml0iXeSaq9XdfU0dRKRyvKH7RP1lg7opbjfRFVJXaNp+M+bNH7cPbpWf2sLN8myFt4LcQgfPcMfHTGO/r1emMUbdKVZzxsGaF0ZsO/yysYb/J97GHuFSF3G0g56ze3kad+rxznqwc+mrqRERCz1n5exbslLDzAvjuB1FwYMuI0Ptsls9ZjnG9idj/21IvoMGJREH8vvo1D7EfmJ8TZuTt4chmmMxYy9wJJrB4keG3N3u5Av11VHVuJzm+ydXNNR3RzW10qnd4FCjCsnskLgX3gwWkKIaCW7zjze2bbhMbsR0yb+t7c7nzCISXSGZ0xacKkU871ZPdcDOsIfMIWDbdGu49ZdB3i4+dc1y+R8vMe6oT3BmZCW/wneN5cH1fyNr0ZC9ZydAKkvxApt87L4yXV5i0TVkR09eTWgtj04O5OvhoLts9vbwsILCTcHdkPwC5WRWyugofrw+Bc5u450Kc6h5r1g3B5pWlAhRUw/KKrT9HLWoaYHqxaWmKOOk9qG2+rY+Nyg1rdfhRTl88YBCaP+xgyny6qOinNt1uzoyDXbq5/UomYo2/08Iy7/x9vYN/14YpHVCUGrZ3prsmFU906YK7tGTLsBs9QuyW5Gq3TCtj4dFdx3HOyZyYzbPeajxTxURL7n08u+MpAyLtoIBT4NqyeMCeT2NIi3OV8CCRFonIAlsh3ZRK7fF18plhlP2+yqF7H6otRyv4hTPJnx5zRmSbx6+N87PxB5/fsVWjCpe4Nvs0rkgV8p9i+Pbd5vckGt/uFUjpuVhvN6mwMJ3GtjS7KM0vdPYwUFgZbhE8mqNc4nZ4V1tZVyYuC3wfNKsSErVUtJZEx8IQvlV56VyMwxKdNWZMNH737UHWpFZmh+uNXmDIFdg48vVV4zWOa28pn1/fCmXbXhuaHm7r3JINNSnrFk+CH1MbdVZG14g8BgB6YbHSMwku5EDju6Pu5IeWlVVlTJ46kxBZoBZuzBi6fVeaw6xFtrjBCeCeKGnS8SDl5eGZIIyM9qazDLyWJ6zlD9kUGNuoMpZLmbqOOsWDRQtjPWUymaXrZ28Ix49P3e3XMzyWqxeAlBVMYxH2HJVOdwLYNtrqcLkYuaXAWwAVQqd3OpK0ALd4NMPPTVFKdMwKwkHtoEqhRb8q0NUGTDhoHv+qILlYfZSCrAdXNID6G40vIQjHuet9LU0khCcaNuym0u8Lz34SWfb+GAA29XUEmWsqbUdq+iwgNWZLapwI7nH6SCRlaBiq2kGw9SSmR2Mt6XASg01gxYQ3ruaGucutcztfdR46aI4JFiaJfEtta0ylu5/jJcnKkFtSB7lBRS9DPf8uNdg1RLLJbA7uhXYGoFXcOOXWYd+BUMe5QXqmKHJ6jNEAmIpO3XIdDACUO2tQYWkbk8EgXGGkEN9E0RnssslIURemhhiviNYXTlicxPRIagHUJdEg61xuH1Urq91OaPm1PFOEexyQ7aZJbuw5WAEoWrpVA/tDgkHy5vxXMcnEVTlQaqUN81np450ASOMDHTP7YAqtFjS7GzIBYq3wR7U71QGxU4MM+uV48xy3qGZ6k5ULBklznjtM7wAXqakZJdYbrK8sy0X2AlyI31DUP3JKEBHWuZyMHiQb9YoJJecoxNktz8c2A/C00sw55qLkvOtA6UBvENoG8FOsXfbyJXjzK4H4aMpcb3a+YqCP0HF2iPKE7GyCSSmtn45TiLF9corQBUiFD4qfeLqwoEKOi+yPhDYMUqxsVK52oQNPLofIjXnXgWwbygEa+cC0XAdcAi4NJsZOSqPRgNHQYpZRUhrl+PkRaKPeGY2KMfJitoakUqpDMsADgbFFVH1Y7RYCxwPdb4iouEU4JCIPmqyHJcLHBTT44QrWwW1wHFRlWcv5Tj5UezHO8VYChwc4fvhzDoDgeMDlqA6hyjAkwBugmrdyWlbgpWgWnly2sbFPXqCqj4zHTxJqKOU0rcSPGEIxOuVaNE5EDx5yCjv7CwvBqMYxShGMYpRjGIUo3Bc/D+m0TMmFAdEyQAAAABJRU5ErkJggg=="/&gt;
-                            &lt;/a&gt;
                             &lt;br/&gt;
                             &lt;span style="font-style:italic;font-size:8pt;font-family:Times New Roman;"&gt;
                                 DSWD-PMB-GF-015 | REV 01 | 30 SEPT 20
@@ -327,12 +318,6 @@
                             &lt;span style="font-size:12pt;font-family:Arial;"&gt;
                                 &lt;p&gt;Date: &lt;t t-out="object.valid_from"/&gt;&lt;/p&gt;
                                 &lt;p&gt;
-                                    &lt;t t-out="object.service_provider_id.name"/&gt;
-                                    &lt;br/&gt;
-                                    &lt;t t-out="object.service_provider_id.address"/&gt;
-                                    &lt;t t-out="object.service_provider_id.city"/&gt;
-                                &lt;/p&gt;
-                                &lt;p&gt;
                                     Dear &lt;span style="font-weight:bold;"&gt;&lt;t t-out="object.service_provider_id.name"/&gt;&lt;/span&gt;,
                                     &lt;br/&gt;
                                     This has reference to the request for the medical assistance of herein client,
@@ -344,37 +329,6 @@
                                     of &lt;t t-out="object.partner_id.address"/&gt;.
                                 &lt;/p&gt;
                                 &lt;p&gt;
-                                    The Department of Social Welfare and Development has assessed and validated
-                                    the said request for assistance through the Crisis Intervention Division.
-                                    Thus, the Department is using this letter to guarantee the payment of
-                                    the bill in the amount of ₱ &lt;t t-out="object.initial_amount"/&gt;
-                                    only.
-                                &lt;/p&gt;
-                                &lt;p&gt;
-                                    To facilitate the payment, please submit to the Crisis Intervention Division
-                                    the following documents for the preparation of Disbursement Voucher within
-                                    one week after service has been completed.
-                                &lt;/p&gt;
-                                &lt;p&gt;
-                                    - Guarantee Letter (GL) from the DSWD with your company's
-                                    "received" stamp. &lt;br/&gt;
-                                    - Statement of Accounts (SOA) or Billing Statement addressed to DSWD.
-                                &lt;/p&gt;
-                                &lt;p&gt;
-                                    Please be informed that said payment will be directly deposited to your
-                                    company's bank account. Should there be any query, you may call us at
-                                    +1 (650) 555-0111.
-                                &lt;/p&gt;
-                                &lt;p&gt;For your consideration.&lt;/p&gt;
-                                &lt;p&gt;Thank You.&lt;/p&gt;
-                                &lt;p&gt;
-                                    Very truly yours,&lt;br/&gt;&lt;br/&gt;
-                                    _______________________&lt;br/&gt;
-                                    Approving Authority&lt;br/&gt;
-                                    Position&lt;br/&gt;
-                                    Office&lt;br/&gt;
-                                &lt;/p&gt;
-                                &lt;p&gt;
                                     &lt;span style="font-weight:bold;"&gt;Valid until:&lt;/span&gt; &lt;t t-out="object.valid_until"/&gt;
                                     &lt;br/&gt;
                                     &lt;span style="font-style:italic;font-size:10pt;font-family:Arial;"&gt;
@@ -383,23 +337,16 @@
                                 &lt;/p&gt;
                             &lt;/span&gt;
                         &lt;/div&gt;
-                        &lt;div style="position:absolute;bottom:1.5in;left:50%;transform: translateX(-50%);"&gt;
-                            &lt;span style="font-weight:bold;font-size:8pt;font-family:Times New Roman;"&gt;
-                                &lt;p&gt;PAGE 1 of 1&lt;/p&gt;
-                            &lt;/span&gt;
-                        &lt;/div&gt;
-                        &lt;div style="position:absolute;bottom:1.2in;left:50%;transform: translateX(-50%);"&gt;
-                            &lt;span style="font-size:8pt;font-family:Times New Roman;"&gt;
-                                &lt;p&gt;DSWD Central/Field Office __ , (address), Philippines (Zip Code)&lt;/p&gt;
-                            &lt;/span&gt;
-                        &lt;/div&gt;
-                        &lt;div style="position:absolute;bottom:1in;left:50%;transform: translateX(-50%);"&gt;
-                            &lt;span style="font-size:8pt;font-family:Times New Roman;"&gt;
-                                &lt;p&gt;Website: &lt;a href="http://www.dswd.gov.ph"&gt;https://www.dswd.gov.ph&lt;/a&gt; Tel Nos.: __________   Telefax: ________&lt;/p&gt;
-                            &lt;/span&gt;
-                        &lt;/div&gt;
-                        &lt;div style="position:absolute;bottom:1in;right:1in"&gt;
-                            &lt;img style="width:1.05in;height:0.6in" src="data:image/jpeg;base64,/9j/4AAQSkZJRgABAQEAYABgAAD/2wBDAAgGBgcGBQgHBwcJCQgKDBQNDAsLDBkSEw8UHRofHh0aHBwgJC4nICIsIxwcKDcpLDAxNDQ0Hyc5PTgyPC4zNDL/2wBDAQkJCQwLDBgNDRgyIRwhMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjIyMjL/wAARCABsAK0DASIAAhEBAxEB/8QAHwAAAQUBAQEBAQEAAAAAAAAAAAECAwQFBgcICQoL/8QAtRAAAgEDAwIEAwUFBAQAAAF9AQIDAAQRBRIhMUEGE1FhByJxFDKBkaEII0KxwRVS0fAkM2JyggkKFhcYGRolJicoKSo0NTY3ODk6Q0RFRkdISUpTVFVWV1hZWmNkZWZnaGlqc3R1dnd4eXqDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uHi4+Tl5ufo6erx8vP09fb3+Pn6/8QAHwEAAwEBAQEBAQEBAQAAAAAAAAECAwQFBgcICQoL/8QAtREAAgECBAQDBAcFBAQAAQJ3AAECAxEEBSExBhJBUQdhcRMiMoEIFEKRobHBCSMzUvAVYnLRChYkNOEl8RcYGRomJygpKjU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6goOEhYaHiImKkpOUlZaXmJmaoqOkpaanqKmqsrO0tba3uLm6wsPExcbHyMnK0tPU1dbX2Nna4uPk5ebn6Onq8vP09fb3+Pn6/9oADAMBAAIRAxEAPwD1HQNC0u60K1nns4nkdMsxHJrU/wCEY0b/AJ8If++ab4WH/FN2X/XOtn27VtVqzVSWr3ODDYak6MG4rZdDI/4RjRv+gfD+VH/CMaN/0D4fyrXxVK91C0sUU3M6ozAlE6u+Bk7VHJOPSo9rP+ZnR9Wo/wAq+4rf8Ixo3/PhD+VH/CMaN/z4Q/lWPL44tlmWO1sZ7jfbpcIw4VgzYxu5XPU4z2P1oh8U6hcyCOHRZ4m8sH/So5EG/ftZMhTzgg5570e0qfzMX1aj/KvuNf8A4RjRv+gfD+VH/CMaN/0D4fyqhN4vtLVmGoRPbBCwkbcGC43kHHUghM5xjkDrW9bXdvexebbTJLHkjchyMjqKPaT/AJmP6tR/lX3FD/hGNG/6B8P5Uv8AwjGjf9A+H/vmtail7Wfdh9Wo/wAq+4599GsNP1GwltrWONzMQWUdtjV0IrO1DP2zT/8Ar4P/AKLetD+GiTbSbClCMG1FWQ+iiipNwpCcDNLTGUMpDAEHgg0AOBB6UZrj9c8FLfu9zpGqXui35HElrKwiY/7Uedp+owa8+1nxn8RvAlwg1uC01KzY4S5EQCv7ZTG0+xHbvVKHNsyJT5d0e40V5Zonxw8PX5SPUoLjTZG6s372MH/eAz+lej2V9aalbrcWV1Dcwt0kicMD+IocXHccZxlsy7RRRUlGJ4W/5Fyy/wCuYrZrG8Lf8i5Zf9c6t6pqFvpOnTX104SKMDJY4GSQAPbJIFXV/iS9Tnwn8CHoipf61Y2lzHYSXsNveXRKQbsNhyPlyM9+2cZxiqGl6Be/a5LzVrpp5GkDLGhGxdpypGACCMsvfKkA9Ki8NadcS3baveyM8siFEYybywLE7uCVAwQAF+XjPWtTXdct9AsGuZ/mY8Rxjq7en/16UYuT5Y7ms5xpxcpOyRetLKz023ENpbQ28IOQkaBR+lWBKh/iFeK6r4t1fVJWLXLwQ9ooTtA+p6msIO4feGYODncDzn1r0oZXNq8pWPEqZ3BStCN0fQMsEFwoWWJHAIYbhnkHI/UZrml8M3GmatBcaZdSJZ/LE9vgZhTduYpngAnGeM43ck4xwGk+MNW0uYZuGuYP4opmz+R6iuzv/H1tJYqdN/eTOPmyOIz6H1NY1MDWhJRWtzop5tQlTc5aW6Hc9aU1xXg3xDNevJZXkpeUfPG7Hlh3H4V2tctalKlPkkduGxMMRTVSGxnah/x+6d/13P8A6LetHtWfqH/H7p3/AF3P/ot60R0qXsjSHxSFoooqTUKKKRjgUAQSypDE8shCogJZj0AFYtgw12Ka8uYQ9hMpigglTIePu5B/vdh6Y9ayL+7bxVrZ0e1Y/wBm27Br6VT98g8RD8Rz+NdlHGscYRAAqjAA7VKd3oazhyRSfxP8EeH/ABB+D32ZJtW8NRs0SjdLYDJI9TH7f7P5eleV6Nr+reHL0XWl3s1rMOGCnhvZlPB/GvskjNfNHxk8P2eieMVmskEcd/D57xgcK+4gkfXr+dddKpze7I4KtPl95Ho3gD4sWviSSPS9WWO01QjCODiOc+gz0b2/L0r1KviSOR4ZVljcpIhDKynBBHQ19ceDdVl1zwbpWo3Me6eaAGQ46sOCfxIzU1aajqi6VRy0ZZ8Lf8i5Zf8AXOqviqVhpRtxcTWrShik8RAKsqlgBkdSRjAwfQ1a8Lf8i5Zf9c6xfG9pbzS6VPcvYbYpWVY7yJWDs23GCWBB+XtnOfas6vxy9RYT+DD0R1Fhb/ZLC2gLZ8uJVJJySQOTXk3jnVJNQ8STRE/ubX90g9+5/P8AlXsKENGCMYI4xXiHiqF4PE+oI4wTKWH0PIrvyyKdZt9EebnUpKiktm9TW8GeFYtaMl7e5NtG21Ywcb275PpXoNxoeiQWTCawtEhVeSY1GB9a574b38B0uay3ATxyFyp7qcc10PiHRBrVj5QmeJ0O5SCdpPuO9Tiqk5Yhxk7JMMLRhHC89OKlKx4p4pW1trx/7LMgtGOFL9QfQZ5x9eaz9GuCLsxZ+WQHj3FaXiu2m0yQWNwmJN272I6ZH1rG0hC2pRnsuSfyr16b0Vnc8CSbpy51Z6nbaLcNba1ZTKSMSqD9CcH+deyqcqDXienoZdRtUGfmlUcfWva0HyD6V5eapc8Wepw637OS6XKWo/8AH7p3/Xc/+i3rRHSs3UP+PzTv+u5/9FvWiK857I+gh8Uh1FJmqtzbyT48u7nt8f8APIJz/wB9Kak1J88cVxfjDxDPC6aHpWX1K6+XKn/VA9z6H/8AXVLxleah4f0+SSPxPeC4lyLeL7PD+p2dBXP6D8P/ABPqEL61N4rmsr+8BJItQXCnvuyNpPt2qJWk+VM6qUPZRVaauunm/wDI9I8N6HHoOkR2qfNJ96Rz1dz1Jq5d6xpmmqWvdQtbYDr5syr/ADNeX33ws8X3xAm8eXUq4xhzIOD14DVnp+z/ACOMz+JPm9rUt/N62jCKVrnHUqznJya1Z0XiD40+G9MSSPTmfU7kZAEQKx593I5H0BrwfxJ4kv8AxTq8mo6g6lyNqIgwsajoor2ey+AmjRbDfavfXBGdwiVYwf0JH511elfC7wlpDpJFpMc8q4Ie6Yyc+uDxn8K1jOENjCUJz3PBvBvw+1fxdeIyQPb6arDzbuRcDb3Cf3j9OnevqHTbK20nTbewtU2W9vGI419AOKsoixqFUAKOAAOBT6yqVHNmtOmoIxfC3/It2X/XMUmv200+lytBNJDNDmVXjQs3AOQuCDkgnof8KXwt/wAi5Zf9c62DRV/iS9TPCfwYeiMHw1fG509baZZI7iBFHlzLtcoR8rFSSR0I5PUGsTx34ak1BF1GyTdcxLiSNRzIvt7iuk0/RrLSriaW2EuZeArysyxrknagJwq5JOB/IDGrxiqpVpUpqcR4jDxr03CfU+e4bmezuRNbyyQzIeGU4Irfbx3r7Wvk/aUDf89RGN/+H6V6Lq/hDSdWcyzW/lznrJEdpP17H8axf+FZab5mftt0Uz935f54r1fr2GqWdWOp4H9m4ui3GjLT1PMbrzNRmZrgvNNIeWPLE1qp4SvtDtRdXUJxL3HOwejehr1bR/CmlaL89vb7pv8AnrIdzfh6fhWzJDHMjRyKrKwwVI4IrOpmS5l7OOiNIZNKVJqpLVnmHgzS2vtYW4I/c2/zE46t2H9fwr1PHy4qnY6fa6bB5FrGI49xbA9TVz+KuHE13XnzHpZfglhKXJu+pQ1D/j703/r4P/ot6uF1DhSwDEZA7mqWo/8AH5p3/Xc/+i3rB8XX/wDZWpaHelyqrdGJ/QqykHP6H8Kwk+WKZ34eDqVJRW//AADrj06Vl65rVroWnSXdy4CqMKvdm7AVPqGpWum6dJeXMoSFF3Ek15FJLqPxE8TLGgeKziPTJIjT1P8AtH/PSsak+XRbs9DBYP2rdSppCO7/AENDw5pt3408QvrmpqfssTfIn8LEdFGew7+9eheIdasvDejT6leFvLiXhEGWc9lA/wA461JGlh4e0TqlvaWseSx7AfzP8zXnHibU5dR0DXtQ1LRtVRzZzRWSSWJCW0ZUgszf3m6k9hx65ujT5dzDHYr2s/dVorRLsjZ+Fvie/wDFOnatqWoP8zX2I4x92JNi4Uf55NZfxo1m70TTdNk06+urW+uJiuYZmUMgHI29OpXnrU3wKiCeBriQdXvXz+CrXNeNPM8W/GnS9ERyILMKrEKDtOPMduQR02jnI4roSXtH2RwNvkXmTeOrzXPBvhnw/eW/iG/j1edVW4iklMiyELuZtrA4wSBjpz0r13w/dz6j4d029u4wlxcW0csq4xhioJ/WvHvE8sXhb4oWL+IF/wCEgt7tFaJ7sfPbAsVwqDCHkZ+7+Ve6AADAGBUz2RVPdjqKKKzNTE8Lf8i5Zf8AXOtnvWP4V/5Fuy/65itjvV1f4kvU58L/AAYeiPPfiPqN5Z/2WLbWI7WEs7XFst6lpPOoAA2SMMDBPIOM1zkPiptVHhyG617U9I0Se1mZ72aRVlnnRyuwygYAxyD3HvXrl1YWl6qrdWsFwFOVEsYfH502XTrKa2S2ltIHt0xtieMFFx0wOgqDoPH4vFuuyeGrKKfWJIdNk1mWybXQo3m2UfK2cYyxyN3bFaWq6xBa/wBiWFp40u30a6u5lvNU+0K7xkKGSLzQMLn1616k1pbva/Zmt4mt9u3yig249MdMVH/Zlh9kNp9htvsuc+T5S7M/7uMUAeRS6hqd34S8U3dr4m1Sa20WVv7PvoptvngqpKuQPn2njPuaseKLm90PQvC4TWtVdb2UyXEjX6xO+YgdvmNw</t>
+	&lt;/main&gt;
+   &lt;/body&gt;
+&lt;/html&gt;
+                       </t>
+  </si>
+  <si>
+    <t>dateOfBirth</t>
+  </si>
+  <si>
+    <t>02/17/2020</t>
   </si>
 </sst>
 </file>
@@ -428,12 +375,18 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -449,12 +402,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -759,7 +715,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -783,11 +739,61 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901552AF-8EF5-49C8-BC60-380B772F2419}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="409.5">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3F8914-FD58-4A8B-9CB0-BEB78A96E3BC}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -801,23 +807,47 @@
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7572FCF-7AED-4618-9D30-1D18DC7CE342}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -842,7 +872,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D2FCFB-88AB-4563-906B-3DA814DFCD12}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -891,7 +921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C889B8-0D34-4DAA-AE23-E715F1FBADFC}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -916,7 +946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79DF6FD-E899-445D-A023-5F9B3A240117}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -947,7 +977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA15282-C1EE-44D8-B879-EF2CFDD3AE34}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -972,7 +1002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7742507-7362-4F7D-8875-36FE26B53481}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -997,12 +1027,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A48F3D9-9103-4D95-9E7A-7DA4613A30F6}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1011,44 +1041,24 @@
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1057,12 +1067,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9875229-B7B8-4D88-84C3-B6C6D6404F04}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1071,108 +1081,19 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5">
-        <v>10000000000</v>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11AD140B-2EBE-490E-BBF4-33E376A43757}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4">
-        <v>10000000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5">
-        <v>10000000000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1203,10 +1124,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1234,6 +1155,45 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11AD140B-2EBE-490E-BBF4-33E376A43757}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3422EA67-90C1-4AD8-8DC6-0C4052B7082B}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1264,7 +1224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637F85CF-E370-426E-B2B6-5E728F865A5F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1289,17 +1249,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBDDDD3-F5D6-48AF-A03C-B541351AD581}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" activeCellId="1" sqref="H11 I8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1315,8 +1279,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1331,6 +1298,9 @@
       </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1338,10 +1308,11 @@
     <hyperlink ref="E2" r:id="rId1" xr:uid="{590D4E7C-644A-4C0F-9D70-FECB4E7C2D42}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904409A-CC43-474C-AE97-F99B0175A6DC}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1368,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DEBD763-20F6-42F6-9F9B-B8EDE0852460}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1380,145 +1351,174 @@
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F1E45DC-5CFB-4148-BD9C-8AAC7381C01D}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00B2349D-0032-41FD-B5E0-DD25407F4044}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
-      <c r="B3">
-        <v>100</v>
+      <c r="B3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="B4">
-        <v>100</v>
+      <c r="B4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F1E45DC-5CFB-4148-BD9C-8AAC7381C01D}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB09658-267B-44C5-B860-23AF15F73A44}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
     <col min="2" max="2" width="33.5703125" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
@@ -1529,10 +1529,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -1540,7 +1540,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
@@ -1562,10 +1562,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -1576,7 +1576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AC84DE-378F-4F00-9E0C-A40CA2F2CC40}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1592,7 +1592,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
@@ -1600,18 +1600,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1620,12 +1620,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE05693-D659-4573-A68D-1E2B20D68F0B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1637,13 +1637,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -1651,13 +1651,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -1665,13 +1665,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -1686,7 +1686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D54B4B9-9621-4B2F-B76F-53305E8F3645}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1705,16 +1705,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1725,19 +1725,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F2">
         <v>123</v>
@@ -1745,19 +1745,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F3">
         <v>123</v>
@@ -1769,54 +1769,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901552AF-8EF5-49C8-BC60-380B772F2419}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" customWidth="1"/>
-    <col min="4" max="4" width="36" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="409.5">
-      <c r="A2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>